<commit_message>
added casefile trials tc, regular e2e tc
</commit_message>
<xml_diff>
--- a/OutputFiles/TC01_Trials_Filter_Diagnosis-AdenoCervix_WebData.xlsx
+++ b/OutputFiles/TC01_Trials_Filter_Diagnosis-AdenoCervix_WebData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t/>
   </si>
@@ -38,7 +38,25 @@
     <t>Race</t>
   </si>
   <si>
-    <t>Ethnicity</t>
+    <t>CTDC-46730</t>
+  </si>
+  <si>
+    <t>NCI-MATCH</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Ado-trastuzumab Emtansine</t>
+  </si>
+  <si>
+    <t>Adenocarcinoma of the cervix</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>UNKNOWN</t>
   </si>
 </sst>
 </file>
@@ -83,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -114,13 +132,31 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>